<commit_message>
Jan 14, 2020 Update
</commit_message>
<xml_diff>
--- a/femba/functions and sim code/functional_simulation_parameters.xlsx
+++ b/femba/functions and sim code/functional_simulation_parameters.xlsx
@@ -120,7 +120,7 @@
     <t xml:space="preserve">parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">list(lambda=c(0.25,0.75), shape=c(1.5,3), scale=c(0.1,5))</t>
+    <t xml:space="preserve">list(lambda=c(0.25,0.75), shape=c(1.1,14), scale=c(0.1,5))</t>
   </si>
   <si>
     <t xml:space="preserve">n_curves</t>
@@ -302,7 +302,7 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.61328125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="17.71484375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.33"/>
@@ -511,10 +511,10 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="17.3828125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.84"/>
@@ -565,7 +565,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>2</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,7 +670,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="17.3828125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.83"/>

</xml_diff>

<commit_message>
Score Function Loss Update
</commit_message>
<xml_diff>
--- a/femba/functions and sim code/functional_simulation_parameters.xlsx
+++ b/femba/functions and sim code/functional_simulation_parameters.xlsx
@@ -114,13 +114,13 @@
     <t xml:space="preserve">distribution</t>
   </si>
   <si>
-    <t xml:space="preserve">rgamma</t>
+    <t xml:space="preserve">rweibullmix</t>
   </si>
   <si>
     <t xml:space="preserve">parameters</t>
   </si>
   <si>
-    <t xml:space="preserve">list(shape=1, scale=4)</t>
+    <t xml:space="preserve">list(lambda=c(0.25,0.75), shape=c(1.1,14), scale=c(0.1,5))</t>
   </si>
   <si>
     <t xml:space="preserve">n_curves</t>
@@ -299,10 +299,10 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="1" sqref="2:3 B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.00390625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.4453125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="42.33"/>
@@ -511,10 +511,10 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.6796875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.07421875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="60.59"/>
@@ -667,10 +667,10 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="2:3 B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.6796875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.07421875" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.83"/>

</xml_diff>